<commit_message>
Added retention visual functionalized adding differences bar
</commit_message>
<xml_diff>
--- a/data/grad_outcomes_ucsd.xlsx
+++ b/data/grad_outcomes_ucsd.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_git\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AABD3F-90AA-45A7-8B42-AB08B7AB722F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB999467-C8DE-4C52-8FAC-2F7785B13ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="630" windowWidth="14400" windowHeight="9570" xr2:uid="{12DE66F5-2E72-D64D-9310-4AA3C0E4C15E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{12DE66F5-2E72-D64D-9310-4AA3C0E4C15E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="year_discrete" sheetId="2" r:id="rId2"/>
-    <sheet name="year_discrete_transfer" sheetId="3" r:id="rId3"/>
+    <sheet name="retention" sheetId="4" r:id="rId2"/>
+    <sheet name="year_discrete" sheetId="2" r:id="rId3"/>
+    <sheet name="year_discrete_transfer" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$94</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">year_discrete!$A$1:$G$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">year_discrete!$A$1:$G$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="41">
   <si>
     <t>N</t>
   </si>
@@ -158,6 +159,12 @@
   </si>
   <si>
     <t>First Gen</t>
+  </si>
+  <si>
+    <t>American Indian</t>
+  </si>
+  <si>
+    <t>International</t>
   </si>
 </sst>
 </file>
@@ -636,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,9 +653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598BCEE0-0764-9741-9D8D-F99F4ED399D8}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -728,22 +735,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>2019</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.68600000000000005</v>
+        <v>2018</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.90500000000000003</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -754,19 +761,19 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E5">
         <v>2018</v>
       </c>
-      <c r="F5" s="6">
-        <v>0.61399999999999999</v>
+      <c r="F5" s="1">
+        <v>0.92900000000000005</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -777,22 +784,22 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="E6">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F6" s="1">
-        <v>0.78600000000000003</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="G6">
-        <v>2581</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -800,22 +807,22 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="E7">
         <v>2018</v>
       </c>
-      <c r="F7">
-        <v>3.51</v>
-      </c>
-      <c r="G7">
-        <v>1045</v>
+      <c r="F7" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -823,22 +830,22 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E8">
-        <v>2017</v>
-      </c>
-      <c r="F8">
-        <v>3.67</v>
+        <v>2018</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.94399999999999995</v>
       </c>
       <c r="G8">
-        <v>2110</v>
+        <v>5022</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -846,19 +853,19 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E9">
-        <v>2014</v>
-      </c>
-      <c r="F9">
-        <v>2.42</v>
+        <v>2018</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.93400000000000005</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -869,88 +876,88 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="E10">
-        <v>2014</v>
-      </c>
-      <c r="F10">
-        <v>4.03</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
+        <v>2018</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="G10">
+        <v>4071</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>2017</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.754</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2017</v>
-      </c>
-      <c r="F12" s="4">
-        <v>3.67</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4144</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2014</v>
-      </c>
-      <c r="F13" s="4">
-        <v>4.05</v>
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.92500000000000004</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
@@ -964,19 +971,19 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <v>2018</v>
       </c>
       <c r="F14" s="1">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
+        <v>0.93</v>
+      </c>
+      <c r="G14">
+        <v>3211</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -987,16 +994,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>2018</v>
       </c>
       <c r="F15" s="1">
-        <v>0.92900000000000005</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
@@ -1004,22 +1011,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E16">
-        <v>2019</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0.58199999999999996</v>
+        <v>2018</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.92300000000000004</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -1030,19 +1037,19 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
       </c>
       <c r="E17">
         <v>2018</v>
       </c>
-      <c r="F17" s="6">
-        <v>0.45200000000000001</v>
+      <c r="F17" s="1">
+        <v>0.93600000000000005</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -1053,22 +1060,22 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F18" s="1">
-        <v>0.64300000000000002</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="G18">
-        <v>1402</v>
+        <v>6708</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1076,65 +1083,65 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>2018</v>
       </c>
-      <c r="F19">
-        <v>3.48</v>
-      </c>
-      <c r="G19">
-        <v>444</v>
+      <c r="F19" s="1">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>2017</v>
-      </c>
-      <c r="F20">
-        <v>3.55</v>
-      </c>
-      <c r="G20">
-        <v>844</v>
+        <v>2019</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>2014</v>
-      </c>
-      <c r="F21">
-        <v>4.3099999999999996</v>
+        <v>2018</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.61399999999999999</v>
       </c>
       <c r="G21" t="s">
         <v>10</v>
@@ -1142,25 +1149,25 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>2014</v>
-      </c>
-      <c r="F22">
-        <v>2.71</v>
-      </c>
-      <c r="G22" t="s">
-        <v>10</v>
+        <v>2017</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="G22">
+        <v>2581</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1168,22 +1175,22 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F23" s="1">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="G23">
-        <v>2564</v>
+        <v>0.754</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1191,19 +1198,19 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E24">
-        <v>2018</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0.94</v>
+        <v>2019</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.58199999999999996</v>
       </c>
       <c r="G24" t="s">
         <v>10</v>
@@ -1217,16 +1224,16 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E25">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F25" s="6">
-        <v>0.56000000000000005</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="G25" t="s">
         <v>10</v>
@@ -1234,30 +1241,30 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E26">
-        <v>2018</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0.42899999999999999</v>
-      </c>
-      <c r="G26" t="s">
-        <v>10</v>
+        <v>2017</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="G26">
+        <v>1402</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -1269,13 +1276,13 @@
         <v>22</v>
       </c>
       <c r="E27">
-        <v>2017</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0.69699999999999995</v>
-      </c>
-      <c r="G27">
-        <v>2360</v>
+        <v>2019</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1283,7 +1290,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
@@ -1294,11 +1301,11 @@
       <c r="E28">
         <v>2018</v>
       </c>
-      <c r="F28">
-        <v>3.51</v>
-      </c>
-      <c r="G28">
-        <v>771</v>
+      <c r="F28" s="6">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1306,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
@@ -1317,31 +1324,31 @@
       <c r="E29">
         <v>2017</v>
       </c>
-      <c r="F29">
-        <v>3.61</v>
+      <c r="F29" s="1">
+        <v>0.69699999999999995</v>
       </c>
       <c r="G29">
-        <v>1554</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E30">
-        <v>2014</v>
-      </c>
-      <c r="F30">
-        <v>4.25</v>
+        <v>2019</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.61699999999999999</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1352,19 +1359,19 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E31">
-        <v>2014</v>
-      </c>
-      <c r="F31">
-        <v>2.77</v>
+        <v>2018</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.54</v>
       </c>
       <c r="G31" t="s">
         <v>10</v>
@@ -1375,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -1384,13 +1391,13 @@
         <v>15</v>
       </c>
       <c r="E32">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F32" s="6">
-        <v>0.94399999999999995</v>
+        <v>0.78600000000000003</v>
       </c>
       <c r="G32">
-        <v>5022</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1398,19 +1405,19 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E33">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F33" s="6">
-        <v>0.93400000000000005</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="G33" t="s">
         <v>10</v>
@@ -1424,16 +1431,16 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E34">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F34" s="6">
-        <v>0.61699999999999999</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="G34" t="s">
         <v>10</v>
@@ -1441,48 +1448,48 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E35">
-        <v>2018</v>
-      </c>
-      <c r="F35" s="6">
-        <v>0.54</v>
-      </c>
-      <c r="G35" t="s">
-        <v>10</v>
+        <v>2017</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="G35">
+        <v>3422</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E36">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="F36" s="6">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="G36">
-        <v>4302</v>
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1490,65 +1497,65 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E37">
         <v>2018</v>
       </c>
-      <c r="F37">
-        <v>3.49</v>
-      </c>
-      <c r="G37">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="F37" s="6">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="G37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16.5">
       <c r="A38" t="s">
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E38">
         <v>2017</v>
       </c>
-      <c r="F38">
-        <v>3.67</v>
-      </c>
-      <c r="G38">
-        <v>3067</v>
+      <c r="F38" s="1">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="G38" s="5">
+        <v>3344</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>2014</v>
-      </c>
-      <c r="F39">
-        <v>4.0599999999999996</v>
+        <v>2019</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0.53200000000000003</v>
       </c>
       <c r="G39" t="s">
         <v>10</v>
@@ -1559,19 +1566,19 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E40">
-        <v>2014</v>
-      </c>
-      <c r="F40">
-        <v>2.58</v>
+        <v>2018</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.434</v>
       </c>
       <c r="G40" t="s">
         <v>10</v>
@@ -1582,42 +1589,42 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="E41">
-        <v>2018</v>
-      </c>
-      <c r="F41" s="2">
-        <v>0.94099999999999995</v>
+        <v>2017</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.71299999999999997</v>
       </c>
       <c r="G41">
-        <v>4071</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E42">
-        <v>2018</v>
-      </c>
-      <c r="F42" s="2">
-        <v>0.93200000000000005</v>
+        <v>2017</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.64251592356687903</v>
       </c>
       <c r="G42" t="s">
         <v>10</v>
@@ -1631,16 +1638,16 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
         <v>38</v>
       </c>
       <c r="E43">
         <v>2019</v>
       </c>
       <c r="F43" s="6">
-        <v>0.61699999999999999</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="G43" t="s">
         <v>10</v>
@@ -1654,16 +1661,16 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
         <v>38</v>
       </c>
       <c r="E44">
         <v>2018</v>
       </c>
       <c r="F44" s="6">
-        <v>0.54700000000000004</v>
+        <v>0.49</v>
       </c>
       <c r="G44" t="s">
         <v>10</v>
@@ -1677,85 +1684,85 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
         <v>38</v>
       </c>
       <c r="E45">
         <v>2017</v>
       </c>
-      <c r="F45" s="2">
-        <v>0.79</v>
+      <c r="F45" s="1">
+        <v>0.69032258064516128</v>
       </c>
       <c r="G45">
-        <v>3422</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E46">
-        <v>2018</v>
-      </c>
-      <c r="F46">
-        <v>3.49</v>
-      </c>
-      <c r="G46">
-        <v>1005</v>
+        <v>2017</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="G46" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>2017</v>
-      </c>
-      <c r="F47">
-        <v>3.69</v>
-      </c>
-      <c r="G47">
-        <v>2435</v>
+        <v>2019</v>
+      </c>
+      <c r="F47" s="6">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>2014</v>
-      </c>
-      <c r="F48">
-        <v>4.04</v>
+        <v>2018</v>
+      </c>
+      <c r="F48" s="6">
+        <v>0.51900000000000002</v>
       </c>
       <c r="G48" t="s">
         <v>10</v>
@@ -1763,48 +1770,48 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>2014</v>
-      </c>
-      <c r="F49">
-        <v>2.62</v>
-      </c>
-      <c r="G49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="16.5">
+        <v>2017</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.75105189340813461</v>
+      </c>
+      <c r="G49">
+        <v>5704</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E50">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F50" s="1">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="G50" s="5">
-        <v>4144</v>
+        <v>0.64341085271317833</v>
+      </c>
+      <c r="G50" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1812,137 +1819,137 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
       </c>
       <c r="E51">
         <v>2018</v>
       </c>
-      <c r="F51" s="1">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="G51" t="s">
-        <v>10</v>
+      <c r="F51">
+        <v>3.51</v>
+      </c>
+      <c r="G51">
+        <v>1045</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <v>2017</v>
+      </c>
+      <c r="F52">
+        <v>3.67</v>
+      </c>
+      <c r="G52">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="4">
+        <v>2017</v>
+      </c>
+      <c r="F53" s="4">
+        <v>3.67</v>
+      </c>
+      <c r="G53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
         <v>11</v>
       </c>
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52">
-        <v>2019</v>
-      </c>
-      <c r="F52" s="6">
-        <v>0.64500000000000002</v>
-      </c>
-      <c r="G52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54">
         <v>2018</v>
       </c>
-      <c r="F53" s="6">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="G53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="16.5">
-      <c r="A54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54">
-        <v>2017</v>
-      </c>
-      <c r="F54" s="1">
-        <v>0.78900000000000003</v>
-      </c>
-      <c r="G54" s="5">
-        <v>3344</v>
+      <c r="F54">
+        <v>3.48</v>
+      </c>
+      <c r="G54">
+        <v>444</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E55">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F55">
-        <v>3.47</v>
+        <v>3.55</v>
       </c>
       <c r="G55">
-        <v>1152</v>
+        <v>844</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E56">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F56">
-        <v>3.66</v>
+        <v>3.51</v>
       </c>
       <c r="G56">
-        <v>2357</v>
+        <v>771</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1950,22 +1957,22 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E57">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="F57">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="G57" t="s">
-        <v>10</v>
+        <v>3.61</v>
+      </c>
+      <c r="G57">
+        <v>1554</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1973,22 +1980,22 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E58">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F58">
-        <v>2.44</v>
-      </c>
-      <c r="G58" t="s">
-        <v>10</v>
+        <v>3.49</v>
+      </c>
+      <c r="G58">
+        <v>1479</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1996,22 +2003,22 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E59">
-        <v>2018</v>
-      </c>
-      <c r="F59" s="1">
-        <v>0.93</v>
+        <v>2017</v>
+      </c>
+      <c r="F59">
+        <v>3.67</v>
       </c>
       <c r="G59">
-        <v>3211</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2019,45 +2026,45 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E60">
         <v>2018</v>
       </c>
-      <c r="F60" s="1">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="G60" t="s">
-        <v>10</v>
+      <c r="F60">
+        <v>3.49</v>
+      </c>
+      <c r="G60">
+        <v>1005</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E61">
-        <v>2019</v>
-      </c>
-      <c r="F61" s="6">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="G61" t="s">
-        <v>10</v>
+        <v>2017</v>
+      </c>
+      <c r="F61">
+        <v>3.69</v>
+      </c>
+      <c r="G61">
+        <v>2435</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2065,22 +2072,22 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E62">
         <v>2018</v>
       </c>
-      <c r="F62" s="7">
-        <v>0.434</v>
-      </c>
-      <c r="G62" t="s">
-        <v>10</v>
+      <c r="F62">
+        <v>3.47</v>
+      </c>
+      <c r="G62">
+        <v>1152</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2088,22 +2095,22 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E63">
         <v>2017</v>
       </c>
-      <c r="F63" s="1">
-        <v>0.71299999999999997</v>
+      <c r="F63">
+        <v>3.66</v>
       </c>
       <c r="G63">
-        <v>2726</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2157,19 +2164,19 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E66">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="F66">
-        <v>4.0999999999999996</v>
+        <v>3.54</v>
       </c>
       <c r="G66" t="s">
         <v>10</v>
@@ -2180,22 +2187,22 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>4</v>
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>38</v>
       </c>
       <c r="E67">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F67">
-        <v>2.75</v>
-      </c>
-      <c r="G67" t="s">
-        <v>10</v>
+        <v>3.47</v>
+      </c>
+      <c r="G67">
+        <v>835</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2203,22 +2210,22 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>38</v>
       </c>
       <c r="E68">
         <v>2017</v>
       </c>
-      <c r="F68" s="1">
-        <v>0.64251592356687903</v>
-      </c>
-      <c r="G68" t="s">
-        <v>10</v>
+      <c r="F68">
+        <v>3.57</v>
+      </c>
+      <c r="G68">
+        <v>1398</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2228,8 +2235,8 @@
       <c r="B69" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>20</v>
+      <c r="C69" t="s">
+        <v>23</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>3</v>
@@ -2237,8 +2244,8 @@
       <c r="E69">
         <v>2017</v>
       </c>
-      <c r="F69">
-        <v>3.54</v>
+      <c r="F69" s="3">
+        <v>3.69</v>
       </c>
       <c r="G69" t="s">
         <v>10</v>
@@ -2246,25 +2253,25 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F70">
-        <v>4.3</v>
-      </c>
-      <c r="G70" t="s">
-        <v>10</v>
+        <v>3.48</v>
+      </c>
+      <c r="G70">
+        <v>1923</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2272,42 +2279,42 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>2018</v>
-      </c>
-      <c r="F71" s="1">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="G71" t="s">
-        <v>10</v>
+        <v>2017</v>
+      </c>
+      <c r="F71">
+        <v>3.64</v>
+      </c>
+      <c r="G71">
+        <v>3911</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
-      </c>
-      <c r="D72" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E72">
-        <v>2018</v>
-      </c>
-      <c r="F72" s="1">
-        <v>0.93600000000000005</v>
+        <v>2017</v>
+      </c>
+      <c r="F72">
+        <v>3.58</v>
       </c>
       <c r="G72" t="s">
         <v>10</v>
@@ -2318,19 +2325,19 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D73" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="E73">
-        <v>2019</v>
-      </c>
-      <c r="F73" s="6">
-        <v>0.59799999999999998</v>
+        <v>2014</v>
+      </c>
+      <c r="F73">
+        <v>2.42</v>
       </c>
       <c r="G73" t="s">
         <v>10</v>
@@ -2338,94 +2345,94 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D74" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="E74">
-        <v>2018</v>
-      </c>
-      <c r="F74" s="6">
-        <v>0.49</v>
+        <v>2014</v>
+      </c>
+      <c r="F74">
+        <v>4.03</v>
       </c>
       <c r="G74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" t="s">
+      <c r="A75" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B75" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" t="s">
-        <v>38</v>
-      </c>
-      <c r="E75">
-        <v>2017</v>
-      </c>
-      <c r="F75" s="1">
-        <v>0.69032258064516128</v>
-      </c>
-      <c r="G75">
-        <v>2170</v>
+      <c r="B75" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="4">
+        <v>2014</v>
+      </c>
+      <c r="F75" s="4">
+        <v>4.05</v>
+      </c>
+      <c r="G75" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E76">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="F76">
-        <v>3.47</v>
-      </c>
-      <c r="G76">
-        <v>835</v>
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="G76" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E77">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="F77">
-        <v>3.57</v>
-      </c>
-      <c r="G77">
-        <v>1398</v>
+        <v>2.71</v>
+      </c>
+      <c r="G77" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2436,16 +2443,16 @@
         <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="E78">
         <v>2014</v>
       </c>
       <c r="F78">
-        <v>4.2</v>
+        <v>4.25</v>
       </c>
       <c r="G78" t="s">
         <v>10</v>
@@ -2459,16 +2466,16 @@
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>38</v>
-      </c>
-      <c r="D79" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="E79">
         <v>2014</v>
       </c>
       <c r="F79">
-        <v>2.58</v>
+        <v>2.77</v>
       </c>
       <c r="G79" t="s">
         <v>10</v>
@@ -2479,19 +2486,19 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E80">
-        <v>2017</v>
-      </c>
-      <c r="F80" s="1">
-        <v>0.81</v>
+        <v>2014</v>
+      </c>
+      <c r="F80">
+        <v>4.0599999999999996</v>
       </c>
       <c r="G80" t="s">
         <v>10</v>
@@ -2499,22 +2506,22 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E81">
-        <v>2017</v>
-      </c>
-      <c r="F81" s="3">
-        <v>3.69</v>
+        <v>2014</v>
+      </c>
+      <c r="F81">
+        <v>2.58</v>
       </c>
       <c r="G81" t="s">
         <v>10</v>
@@ -2528,16 +2535,16 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E82">
-        <v>2017</v>
-      </c>
-      <c r="F82" s="3">
-        <v>4.07</v>
+        <v>2014</v>
+      </c>
+      <c r="F82">
+        <v>4.04</v>
       </c>
       <c r="G82" t="s">
         <v>10</v>
@@ -2545,45 +2552,45 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="E83">
-        <v>2018</v>
-      </c>
-      <c r="F83" s="1">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="G83">
-        <v>6708</v>
+        <v>2014</v>
+      </c>
+      <c r="F83">
+        <v>2.62</v>
+      </c>
+      <c r="G83" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E84">
-        <v>2018</v>
-      </c>
-      <c r="F84" s="1">
-        <v>0.93300000000000005</v>
+        <v>2014</v>
+      </c>
+      <c r="F84">
+        <v>4.0199999999999996</v>
       </c>
       <c r="G84" t="s">
         <v>10</v>
@@ -2594,19 +2601,19 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E85">
-        <v>2019</v>
-      </c>
-      <c r="F85" s="6">
-        <v>0.60799999999999998</v>
+        <v>2014</v>
+      </c>
+      <c r="F85">
+        <v>2.44</v>
       </c>
       <c r="G85" t="s">
         <v>10</v>
@@ -2614,22 +2621,22 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E86">
-        <v>2018</v>
-      </c>
-      <c r="F86" s="6">
-        <v>0.51900000000000002</v>
+        <v>2014</v>
+      </c>
+      <c r="F86">
+        <v>4.0999999999999996</v>
       </c>
       <c r="G86" t="s">
         <v>10</v>
@@ -2637,48 +2644,48 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E87">
-        <v>2017</v>
-      </c>
-      <c r="F87" s="1">
-        <v>0.75105189340813461</v>
-      </c>
-      <c r="G87">
-        <v>5704</v>
+        <v>2014</v>
+      </c>
+      <c r="F87">
+        <v>2.75</v>
+      </c>
+      <c r="G87" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E88">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="F88">
-        <v>3.48</v>
-      </c>
-      <c r="G88">
-        <v>1923</v>
+        <v>4.3</v>
+      </c>
+      <c r="G88" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2686,42 +2693,42 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="D89" t="s">
+        <v>38</v>
       </c>
       <c r="E89">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="F89">
-        <v>3.64</v>
-      </c>
-      <c r="G89">
-        <v>3911</v>
+        <v>4.2</v>
+      </c>
+      <c r="G89" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="D90" t="s">
+        <v>38</v>
       </c>
       <c r="E90">
         <v>2014</v>
       </c>
       <c r="F90">
-        <v>4.0999999999999996</v>
+        <v>2.58</v>
       </c>
       <c r="G90" t="s">
         <v>10</v>
@@ -2729,22 +2736,22 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B91" t="s">
         <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E91">
-        <v>2014</v>
-      </c>
-      <c r="F91">
-        <v>2.6</v>
+        <v>2017</v>
+      </c>
+      <c r="F91" s="3">
+        <v>4.07</v>
       </c>
       <c r="G91" t="s">
         <v>10</v>
@@ -2755,19 +2762,19 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>2017</v>
-      </c>
-      <c r="F92" s="1">
-        <v>0.64341085271317833</v>
+        <v>2014</v>
+      </c>
+      <c r="F92">
+        <v>4.0999999999999996</v>
       </c>
       <c r="G92" t="s">
         <v>10</v>
@@ -2775,22 +2782,22 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E93">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="F93">
-        <v>3.58</v>
+        <v>2.6</v>
       </c>
       <c r="G93" t="s">
         <v>10</v>
@@ -2828,7 +2835,7 @@
   </sheetData>
   <autoFilter ref="A1:G94" xr:uid="{598BCEE0-0764-9741-9D8D-F99F4ED399D8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G126">
-    <sortCondition descending="1" ref="C2:C126"/>
+    <sortCondition descending="1" ref="B2:B126"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2836,6 +2843,791 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3533A5D2-A182-4C7C-B5A6-2D94B2471668}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="2" max="2" width="11.9140625" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="16.08203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2018</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="F2">
+        <v>6708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>2018</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="F4">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2018</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="F5">
+        <v>3211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="F6">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>2018</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="F8">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>2018</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F9">
+        <v>5022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>2018</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2021</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.93299999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>2021</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.91799999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>2021</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>2021</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>2021</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2021</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="F16">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>2021</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.96700000000000008</v>
+      </c>
+      <c r="F17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2021</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>2021</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>2021</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="F20">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>2021</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.92599999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2018</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>2018</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24">
+        <v>2018</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>2018</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2018</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>2018</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>2018</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>2018</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>2018</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2021</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.92200000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>2021</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.92799999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33">
+        <v>2021</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.92799999999999994</v>
+      </c>
+      <c r="F33">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>2021</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="F34">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35">
+        <v>2021</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="F35">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>2021</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="F36">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>2021</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="F37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>2021</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="F38">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>2021</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.90799999999999992</v>
+      </c>
+      <c r="F39">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>2021</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="F40">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>2021</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="F41">
+        <v>765</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
+    <sortCondition ref="A2:A31"/>
+    <sortCondition ref="D2:D31"/>
+    <sortCondition ref="C2:C31"/>
+    <sortCondition ref="B2:B31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC7ECB2-5042-405F-975F-571C504B6DEC}">
   <dimension ref="A1:G211"/>
   <sheetViews>
@@ -7704,7 +8496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCB52AE-C55F-488D-BDEC-82D4BD065CAE}">
   <dimension ref="A1:Q101"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added in doctoral completion
</commit_message>
<xml_diff>
--- a/data/grad_outcomes_ucsd.xlsx
+++ b/data/grad_outcomes_ucsd.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB999467-C8DE-4C52-8FAC-2F7785B13ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75634E1A-34A0-4DB0-928D-990D52F2E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{12DE66F5-2E72-D64D-9310-4AA3C0E4C15E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="retention" sheetId="4" r:id="rId2"/>
-    <sheet name="year_discrete" sheetId="2" r:id="rId3"/>
-    <sheet name="year_discrete_transfer" sheetId="3" r:id="rId4"/>
+    <sheet name="GPA" sheetId="5" r:id="rId2"/>
+    <sheet name="retention" sheetId="4" r:id="rId3"/>
+    <sheet name="year_discrete" sheetId="2" r:id="rId4"/>
+    <sheet name="year_discrete_transfer" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$94</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">year_discrete!$A$1:$G$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">year_discrete!$A$1:$G$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="42">
   <si>
     <t>N</t>
   </si>
@@ -165,6 +166,9 @@
   </si>
   <si>
     <t>International</t>
+  </si>
+  <si>
+    <t>exitcohort</t>
   </si>
 </sst>
 </file>
@@ -654,8 +658,8 @@
   <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -2843,11 +2847,140 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A694BB2-5FE9-4554-9778-AFECF20EEF0D}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="13.08203125" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3533A5D2-A182-4C7C-B5A6-2D94B2471668}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -3627,7 +3760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC7ECB2-5042-405F-975F-571C504B6DEC}">
   <dimension ref="A1:G211"/>
   <sheetViews>
@@ -8496,7 +8629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCB52AE-C55F-488D-BDEC-82D4BD065CAE}">
   <dimension ref="A1:Q101"/>
   <sheetViews>

</xml_diff>

<commit_message>
More updates to tables, questiosn
</commit_message>
<xml_diff>
--- a/data/grad_outcomes_ucsd.xlsx
+++ b/data/grad_outcomes_ucsd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75634E1A-34A0-4DB0-928D-990D52F2E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A54A500-34D1-4FA3-B83A-0C479BE51432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{12DE66F5-2E72-D64D-9310-4AA3C0E4C15E}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="50">
   <si>
     <t>N</t>
   </si>
@@ -170,6 +170,30 @@
   <si>
     <t>exitcohort</t>
   </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>&gt;3.49</t>
+  </si>
+  <si>
+    <t>3.00-3.49</t>
+  </si>
+  <si>
+    <t>2.5-2.99</t>
+  </si>
+  <si>
+    <t>2.00-2.49</t>
+  </si>
+  <si>
+    <t>Applicant Type</t>
+  </si>
+  <si>
+    <t>FTFY</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
 </sst>
 </file>
 
@@ -275,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -340,6 +364,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2848,32 +2875,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A694BB2-5FE9-4554-9778-AFECF20EEF0D}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" customWidth="1"/>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
@@ -2883,91 +2911,702 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2">
+        <v>0.54</v>
+      </c>
+      <c r="F2">
+        <v>3018</v>
       </c>
     </row>
     <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>2022</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="F3">
+        <v>1860</v>
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>0.109</v>
+      </c>
+      <c r="F4">
+        <v>608</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="F6">
+        <v>1327</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>0.34</v>
+      </c>
+      <c r="F7">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>2022</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>0.152</v>
+      </c>
+      <c r="F8">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="4" t="s">
+      <c r="C10">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>0.373</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="F11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <v>0.224</v>
+      </c>
+      <c r="F12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="4" t="s">
+      <c r="C14">
+        <v>2022</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="F14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>2022</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>2022</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="4" t="s">
+      <c r="C18">
+        <v>2022</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="F18">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>2022</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="F19">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>2022</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20">
+        <v>0.105</v>
+      </c>
+      <c r="F20">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>2022</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="B11" s="4" t="s">
+      <c r="C22">
+        <v>2022</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="F22">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>2022</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F23">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>2022</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F24">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="B12" s="4" t="s">
+      <c r="C26">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="F26">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>2022</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="F27">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>2022</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="F28">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>2022</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
         <v>7</v>
+      </c>
+      <c r="C30">
+        <v>2022</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="F30">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>2022</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="F31">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>2022</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F32">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>2022</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>2022</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F34">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>2022</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F35">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>2022</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36">
+        <v>0.123</v>
+      </c>
+      <c r="F36">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>2022</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="F37">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>